<commit_message>
test: 💍 update and refactor test for import and exportexcel fil
</commit_message>
<xml_diff>
--- a/tests/stubs/products.xlsx
+++ b/tests/stubs/products.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ladycath\php\eCommerce-2\tests\stubs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57837A-7124-4A0C-BEA9-E8D0C1CE2454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="2180" yWindow="400" windowWidth="14400" windowHeight="5680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="181029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +65,6 @@
     <t>Culpa aut vel ut voluptates blanditiis.</t>
   </si>
   <si>
-    <t>sit</t>
-  </si>
-  <si>
     <t>dolorum</t>
   </si>
   <si>
@@ -68,18 +80,12 @@
     <t>Inventore nihil repellat expedita enim optio.</t>
   </si>
   <si>
-    <t>rerum</t>
-  </si>
-  <si>
     <t>incidunt</t>
   </si>
   <si>
     <t>Possimus quam cumque quisquam nihil ut optio.</t>
   </si>
   <si>
-    <t>nobis</t>
-  </si>
-  <si>
     <t>nihil</t>
   </si>
   <si>
@@ -98,9 +104,6 @@
     <t>Dolores officia et eaque autem eum ut.</t>
   </si>
   <si>
-    <t>ut</t>
-  </si>
-  <si>
     <t>aut</t>
   </si>
   <si>
@@ -123,9 +126,6 @@
   </si>
   <si>
     <t>Nobis modi molestiae ut et quod itaque.</t>
-  </si>
-  <si>
-    <t>quae</t>
   </si>
   <si>
     <t>consectetur</t>
@@ -182,14 +182,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -204,21 +199,33 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -508,19 +515,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I2:I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -560,13 +564,13 @@
         <v>10426</v>
       </c>
       <c r="D2">
-        <v>311458.0</v>
+        <v>311458</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>5453</v>
@@ -575,53 +579,53 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>525703</v>
       </c>
       <c r="D3">
-        <v>315868.0</v>
+        <v>315868</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>6780</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>132948</v>
       </c>
       <c r="D4">
-        <v>738559.0</v>
+        <v>738559</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="G4">
         <v>1958</v>
@@ -630,27 +634,27 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>223303</v>
       </c>
       <c r="D5">
-        <v>651992.0</v>
+        <v>651992</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>3430</v>
@@ -659,53 +663,53 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>554298</v>
       </c>
       <c r="D6">
-        <v>651114.0</v>
+        <v>651114</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="G6">
         <v>1695</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>494908</v>
       </c>
       <c r="D7">
-        <v>530605.0</v>
+        <v>530605</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>6053</v>
@@ -714,53 +718,53 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>454460</v>
       </c>
       <c r="D8">
-        <v>130297.0</v>
+        <v>130297</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>2250</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>201065</v>
       </c>
       <c r="D9">
-        <v>34699.0</v>
+        <v>34699</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="G9">
         <v>108</v>
@@ -769,27 +773,27 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>937696</v>
       </c>
       <c r="D10">
-        <v>784567.0</v>
+        <v>784567</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="G10">
         <v>8759</v>
@@ -798,27 +802,27 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>465051</v>
       </c>
       <c r="D11">
-        <v>257973.0</v>
+        <v>257973</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="G11">
         <v>5889</v>
@@ -827,27 +831,27 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>162226</v>
       </c>
       <c r="D12">
-        <v>325094.0</v>
+        <v>325094</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F12">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="G12">
         <v>2120</v>
@@ -856,105 +860,105 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>111683</v>
       </c>
       <c r="D13">
-        <v>738470.0</v>
+        <v>738470</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F13">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="G13">
         <v>5374</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>824356</v>
       </c>
       <c r="D14">
-        <v>837361.0</v>
+        <v>837361</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F14">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="G14">
         <v>1682</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>363728</v>
       </c>
       <c r="D15">
-        <v>850614.0</v>
+        <v>850614</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F15">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="G15">
         <v>9577</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>827430</v>
       </c>
       <c r="D16">
-        <v>763766.0</v>
+        <v>763766</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F16">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="G16">
         <v>8934</v>
@@ -963,27 +967,27 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>422394</v>
       </c>
       <c r="D17">
-        <v>34569.0</v>
+        <v>34569</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F17">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="G17">
         <v>6880</v>
@@ -992,79 +996,79 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <v>527290</v>
       </c>
       <c r="D18">
-        <v>194457.0</v>
+        <v>194457</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F18">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="G18">
         <v>7776</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>68194</v>
       </c>
       <c r="D19">
-        <v>435204.0</v>
+        <v>435204</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F19">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="G19">
         <v>8545</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>284273</v>
       </c>
       <c r="D20">
-        <v>758009.0</v>
+        <v>758009</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F20">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>7609</v>
@@ -1073,27 +1077,27 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>20801</v>
       </c>
       <c r="D21">
-        <v>830842.0</v>
+        <v>830842</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F21">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="G21">
         <v>2560</v>
@@ -1102,21 +1106,11 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>